<commit_message>
created import function, tested simon munzert repo, created CSV
</commit_message>
<xml_diff>
--- a/data/raw/Project Management Assignments (Contract Tracker)_repo_check.xlsx
+++ b/data/raw/Project Management Assignments (Contract Tracker)_repo_check.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/Documents/08 - Hertie/thesis_stf/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B49A329-08CB-1544-81CD-6D16F92C0BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DAAA54-5440-5D44-837B-237212EEECA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20620" yWindow="4340" windowWidth="28560" windowHeight="18500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12440" yWindow="800" windowWidth="28560" windowHeight="18500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="162">
   <si>
     <t>Name</t>
   </si>
@@ -493,12 +493,39 @@
   <si>
     <t>https://github.com/sequoia-pgp</t>
   </si>
+  <si>
+    <t>https://github.com/fortran-lang/registry ; https://github.com/fortran-lang/fpm</t>
+  </si>
+  <si>
+    <t>(https://github.com/openmls/openmls</t>
+  </si>
+  <si>
+    <t>https://gitlab.com/sequoia-pgp/sequoia-git</t>
+  </si>
+  <si>
+    <t>https://github.com/openpgpjs/openpgpjs/</t>
+  </si>
+  <si>
+    <t>https://github.com/openbsd/src/</t>
+  </si>
+  <si>
+    <t>https://github.com/rubygems/rubygems</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>https://github.com/curl/curl/</t>
+  </si>
+  <si>
+    <t>https://github.com/pendulum-project/ntpd-rs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -518,6 +545,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -544,27 +586,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -596,54 +630,46 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -656,6 +682,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A5BB8C01-2BAA-C64E-866C-CD7A103999B2}" name="Table1" displayName="Table1" ref="A1:M35" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:M35" xr:uid="{A5BB8C01-2BAA-C64E-866C-CD7A103999B2}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{701730A1-60CF-A943-8244-6C6745408A1C}" name="Github Repo?"/>
+    <tableColumn id="2" xr3:uid="{4ED4471E-E62C-D241-86E6-CDCE403767DB}" name="repo"/>
+    <tableColumn id="3" xr3:uid="{8533C15B-8592-D248-B3AC-69FD6CFB17D0}" name="comment" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{8D1ADDC1-D891-1A40-9A22-67E0F6C1E499}" name="Name"/>
+    <tableColumn id="5" xr3:uid="{A515C0BC-000E-F34F-9C97-9A8BE29DB160}" name="PM"/>
+    <tableColumn id="6" xr3:uid="{FFC97404-31D4-A247-9D50-42527DA9C8F7}" name="Status"/>
+    <tableColumn id="7" xr3:uid="{4B9B6D5B-A7BB-7645-9438-2D323743437D}" name="Total.Amount"/>
+    <tableColumn id="8" xr3:uid="{128B143F-B147-5840-97D8-48A5EEA97C30}" name="Unpaid.Amount"/>
+    <tableColumn id="9" xr3:uid="{5176F984-BA81-E54E-8D31-F465E89D7FCD}" name="Start.Date" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{1CC30C35-62B0-4B41-9A77-87A3C97C55EC}" name="End.Date" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{D91CA4B8-CB6A-0449-AC29-1A98A0F95B80}" name="Tags"/>
+    <tableColumn id="12" xr3:uid="{A2DF0A36-7DB7-0841-A3C6-C708C72E3FED}" name="invoice.check..confirmation.received."/>
+    <tableColumn id="13" xr3:uid="{8E10225F-B902-1A40-8309-4318F9F55F37}" name="Deviation"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -937,26 +985,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="44.6640625" customWidth="1"/>
-    <col min="3" max="3" width="54" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" customWidth="1"/>
-    <col min="7" max="7" width="124.5" customWidth="1"/>
-    <col min="8" max="8" width="37.6640625" customWidth="1"/>
-    <col min="9" max="9" width="42" customWidth="1"/>
-    <col min="10" max="10" width="32.83203125" customWidth="1"/>
-    <col min="11" max="11" width="37.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" customWidth="1"/>
+    <col min="4" max="4" width="54" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" customWidth="1"/>
+    <col min="8" max="8" width="124.5" customWidth="1"/>
+    <col min="9" max="9" width="37.6640625" customWidth="1"/>
+    <col min="10" max="10" width="42" customWidth="1"/>
+    <col min="11" max="11" width="32.83203125" customWidth="1"/>
+    <col min="12" max="12" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>137</v>
       </c>
@@ -964,1216 +1013,1331 @@
         <v>139</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>138</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2">
         <v>136000</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>17</v>
       </c>
-      <c r="L2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>143</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3">
         <v>203000</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
       <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s">
         <v>23</v>
       </c>
-      <c r="L3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>138</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4">
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4">
         <v>455000</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J4" t="s">
-        <v>18</v>
-      </c>
       <c r="K4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" t="s">
         <v>23</v>
       </c>
-      <c r="L4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>143</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5">
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5">
         <v>278700</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J5" t="s">
-        <v>18</v>
-      </c>
       <c r="K5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" t="s">
         <v>23</v>
       </c>
-      <c r="L5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>140</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>31</v>
       </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6">
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6">
         <v>485200</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J6" t="s">
-        <v>18</v>
-      </c>
       <c r="K6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" t="s">
         <v>17</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>138</v>
       </c>
       <c r="B7" t="s">
         <v>145</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" t="s">
         <v>35</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>31</v>
       </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7">
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7">
         <v>1000000</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J7" t="s">
-        <v>18</v>
-      </c>
       <c r="K7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" t="s">
         <v>17</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>138</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" t="s">
         <v>38</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8">
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8">
         <v>596160</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>16</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>23</v>
       </c>
-      <c r="L8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>138</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" t="s">
         <v>41</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>31</v>
       </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9">
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9">
         <v>454350</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J9" t="s">
-        <v>18</v>
-      </c>
       <c r="K9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" t="s">
         <v>17</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>143</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" t="s">
         <v>45</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>46</v>
       </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10">
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10">
         <v>1557468.48</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>49</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>17</v>
       </c>
-      <c r="L10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>143</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4"/>
+      <c r="D11" t="s">
         <v>50</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>31</v>
       </c>
-      <c r="E11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11">
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11">
         <v>152000</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J11" t="s">
-        <v>18</v>
-      </c>
       <c r="K11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" t="s">
         <v>17</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>138</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4"/>
+      <c r="D12" t="s">
         <v>55</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>11</v>
       </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12">
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12">
         <v>99060</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>56</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J12" t="s">
-        <v>18</v>
-      </c>
       <c r="K12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" t="s">
         <v>23</v>
       </c>
-      <c r="L12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>143</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" t="s">
         <v>58</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>31</v>
       </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13">
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13">
         <v>993600</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>59</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J13" t="s">
-        <v>18</v>
-      </c>
       <c r="K13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" t="s">
         <v>17</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>141</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5"/>
+      <c r="D14" t="s">
         <v>62</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>11</v>
       </c>
-      <c r="E14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14">
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14">
         <v>612000</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>63</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>16</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>23</v>
       </c>
-      <c r="L14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>143</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="4"/>
+      <c r="D15" t="s">
         <v>65</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>46</v>
       </c>
-      <c r="E15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15">
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15">
         <v>874940</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>66</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>49</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>23</v>
       </c>
-      <c r="L15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>138</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="4"/>
+      <c r="D16" t="s">
         <v>68</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>69</v>
       </c>
-      <c r="E16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16">
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16">
         <v>263000</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>70</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>49</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>17</v>
       </c>
-      <c r="L16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>143</v>
       </c>
       <c r="B17" t="s">
         <v>152</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="5"/>
+      <c r="D17" t="s">
         <v>71</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>11</v>
       </c>
-      <c r="E17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17">
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17">
         <v>900000</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>72</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="J17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>16</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>17</v>
       </c>
-      <c r="L17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
+      <c r="M17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" t="s">
         <v>74</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>69</v>
       </c>
-      <c r="E18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18">
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18">
         <v>205000</v>
       </c>
-      <c r="G18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="J18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J18" t="s">
-        <v>18</v>
-      </c>
       <c r="K18" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" t="s">
         <v>23</v>
       </c>
-      <c r="L18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>140</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="5"/>
+      <c r="D19" t="s">
         <v>76</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>31</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>77</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>209000</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>78</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="J19" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>81</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>17</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" t="s">
         <v>83</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>46</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>77</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>200000</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>84</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="J20" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>81</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>17</v>
       </c>
-      <c r="L20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
+      <c r="M20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" t="s">
+        <v>154</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" t="s">
         <v>87</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>46</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>77</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>195000</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>88</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>91</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>17</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C22" t="s">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" t="s">
         <v>92</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>46</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>77</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>200000</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>93</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="J22" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>96</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>17</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" t="s">
         <v>97</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>46</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>77</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>172860</v>
       </c>
-      <c r="G23" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>91</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>17</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>143</v>
+      </c>
+      <c r="B24" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" t="s">
         <v>100</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>31</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>77</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>200000</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>101</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="I24" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="J24" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>81</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>17</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" t="s">
         <v>102</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>31</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>77</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>200000</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>103</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="J25" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>81</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>17</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C26" t="s">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" t="s">
         <v>106</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>46</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>107</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>200000</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>108</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="J26" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>111</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>23</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C27" t="s">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" t="s">
         <v>113</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>31</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>77</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>195000</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>114</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="J27" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>81</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>17</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C28" t="s">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>143</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" t="s">
         <v>115</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>69</v>
       </c>
-      <c r="E28" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28">
+      <c r="F28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28">
         <v>349875</v>
       </c>
-      <c r="G28" t="s">
-        <v>18</v>
-      </c>
-      <c r="H28" s="2" t="s">
+      <c r="H28" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="J28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J28" t="s">
-        <v>18</v>
-      </c>
       <c r="K28" t="s">
+        <v>18</v>
+      </c>
+      <c r="L28" t="s">
         <v>23</v>
       </c>
-      <c r="L28" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C29" t="s">
+      <c r="M28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>143</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" t="s">
         <v>116</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>69</v>
       </c>
-      <c r="E29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29">
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29">
         <v>180000</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>117</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="J29" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>49</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>23</v>
       </c>
-      <c r="L29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C30" t="s">
+      <c r="M29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" t="s">
         <v>118</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>69</v>
       </c>
-      <c r="E30" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30">
+      <c r="F30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30">
         <v>668400</v>
       </c>
-      <c r="G30" t="s">
-        <v>18</v>
-      </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="J30" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>16</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>17</v>
       </c>
-      <c r="L30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C31" t="s">
+      <c r="M30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>143</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" t="s">
         <v>120</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>31</v>
       </c>
-      <c r="E31" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31">
+      <c r="F31" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31">
         <v>353430</v>
       </c>
-      <c r="G31" t="s">
-        <v>18</v>
-      </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="J31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J31" t="s">
-        <v>18</v>
-      </c>
       <c r="K31" t="s">
+        <v>18</v>
+      </c>
+      <c r="L31" t="s">
         <v>23</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C32" t="s">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>140</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" t="s">
         <v>123</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>11</v>
       </c>
-      <c r="E32" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32">
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32">
         <v>769829.4</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>124</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="J32" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>16</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>17</v>
       </c>
-      <c r="L32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C33" t="s">
+      <c r="M32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" t="s">
         <v>127</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>31</v>
       </c>
-      <c r="E33" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33">
+      <c r="F33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33">
         <v>1056672.77</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>128</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="I33" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="J33" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>49</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>17</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C34" t="s">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>138</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" t="s">
         <v>131</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>69</v>
       </c>
-      <c r="E34" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34">
+      <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34">
         <v>449850</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>132</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="I34" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="J34" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>16</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>17</v>
       </c>
-      <c r="L34" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C35" t="s">
+      <c r="M34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35" s="5"/>
+      <c r="D35" t="s">
         <v>135</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>69</v>
       </c>
-      <c r="E35" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35">
+      <c r="F35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35">
         <v>205000</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>136</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="I35" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="J35" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J35" t="s">
-        <v>18</v>
-      </c>
       <c r="K35" t="s">
+        <v>18</v>
+      </c>
+      <c r="L35" t="s">
         <v>23</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A35">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="?">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="?">
       <formula>NOT(ISERROR(SEARCH("?",A2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -2185,8 +2349,17 @@
     <hyperlink ref="B12" r:id="rId6" xr:uid="{FC5DF6A9-BD96-2D40-85F0-AB735BC3D0A0}"/>
     <hyperlink ref="B15" r:id="rId7" xr:uid="{93C88F81-F17B-8047-B773-C37EFAAF59E2}"/>
     <hyperlink ref="B16" r:id="rId8" xr:uid="{727AA105-7613-5F4E-9144-560562D7C4CB}"/>
+    <hyperlink ref="B22" r:id="rId9" xr:uid="{5BC7833C-7DA1-904F-96AE-8C2A0130EA8A}"/>
+    <hyperlink ref="B23" r:id="rId10" xr:uid="{4004E30F-959F-6D4E-9EBD-2F2DCE86F20E}"/>
+    <hyperlink ref="B25" r:id="rId11" xr:uid="{1C393B49-FC3D-E349-90A9-142F77FBC5B9}"/>
+    <hyperlink ref="B27" r:id="rId12" xr:uid="{DB3F3E59-7DD7-F74A-A11A-18615C39287F}"/>
+    <hyperlink ref="B30" r:id="rId13" xr:uid="{20C0A362-EDC4-444E-AC0A-9A4A0020E769}"/>
+    <hyperlink ref="B34" r:id="rId14" xr:uid="{78E41816-6B5A-EA41-9AE6-082CCB133245}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
+    <tablePart r:id="rId15"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>